<commit_message>
Changes done to resolve Issues
</commit_message>
<xml_diff>
--- a/GaneshSoley/Supplier_Onboarding/Data/Config.xlsx
+++ b/GaneshSoley/Supplier_Onboarding/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -142,16 +142,7 @@
     <t>GaneshSoley</t>
   </si>
   <si>
-    <t>ImgFileName</t>
-  </si>
-  <si>
-    <t>ExtName</t>
-  </si>
-  <si>
     <t>This value will be used for saving Excel file. This name of the Excel will start with this value. This will not contain any special character</t>
-  </si>
-  <si>
-    <t>This value will be used for saving screenshot file. This name of the image will start with this value.  This will not contain any special character</t>
   </si>
   <si>
     <t>ReceiverMailID</t>
@@ -550,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -558,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -637,7 +628,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -648,7 +639,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -659,7 +650,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -670,31 +661,21 @@
         <v>39</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1681,12 +1662,11 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Code improved to resolve minor issues
</commit_message>
<xml_diff>
--- a/GaneshSoley/Supplier_Onboarding/Data/Config.xlsx
+++ b/GaneshSoley/Supplier_Onboarding/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,24 @@
   </si>
   <si>
     <t>Input File Path from where input data will be read.</t>
+  </si>
+  <si>
+    <t>MailCredential</t>
+  </si>
+  <si>
+    <t>Robot will use this value to access mail Credential details from Orchestrator and use them to send mail.</t>
+  </si>
+  <si>
+    <t>GaneshSoley_GMail</t>
+  </si>
+  <si>
+    <t>Data\Input\MailBody.txt</t>
+  </si>
+  <si>
+    <t>MailBodyTemplate</t>
+  </si>
+  <si>
+    <t>This template is used in mail to send to the stakeholders.</t>
   </si>
 </sst>
 </file>
@@ -541,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,7 +570,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -675,8 +693,28 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
#124 Supply Chain Mgmt PO Tracking Project loaded (#138)
* Test Document

* Create Sales Opportunity PDD

Co-Authored-By: Vajrang <vajrang@outlook.com>

* Create Vajrang IT Services PDD

Co-Authored-By: Vajrang <vajrang@outlook.com>

* Supplier Onboarding

This Project is for Supplier Onboarding

* Code is fixed with screenshot

* Changes done to resolve Issues

* Code improved to resolve minor issues

* SCM Project

Co-authored-by: gsoley <72097981+gsoley@users.noreply.github.com>
Co-authored-by: Vajrang <vajrang@outlook.com>
</commit_message>
<xml_diff>
--- a/GaneshSoley/Supplier_Onboarding/Data/Config.xlsx
+++ b/GaneshSoley/Supplier_Onboarding/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -142,18 +142,9 @@
     <t>GaneshSoley</t>
   </si>
   <si>
-    <t>ImgFileName</t>
-  </si>
-  <si>
-    <t>ExtName</t>
-  </si>
-  <si>
     <t>This value will be used for saving Excel file. This name of the Excel will start with this value. This will not contain any special character</t>
   </si>
   <si>
-    <t>This value will be used for saving screenshot file. This name of the image will start with this value.  This will not contain any special character</t>
-  </si>
-  <si>
     <t>ReceiverMailID</t>
   </si>
   <si>
@@ -170,6 +161,24 @@
   </si>
   <si>
     <t>Input File Path from where input data will be read.</t>
+  </si>
+  <si>
+    <t>MailCredential</t>
+  </si>
+  <si>
+    <t>Robot will use this value to access mail Credential details from Orchestrator and use them to send mail.</t>
+  </si>
+  <si>
+    <t>GaneshSoley_GMail</t>
+  </si>
+  <si>
+    <t>Data\Input\MailBody.txt</t>
+  </si>
+  <si>
+    <t>MailBodyTemplate</t>
+  </si>
+  <si>
+    <t>This template is used in mail to send to the stakeholders.</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -637,7 +646,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -648,7 +657,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -659,7 +668,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -670,15 +679,15 @@
         <v>39</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>43</v>
@@ -686,16 +695,26 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1681,12 +1700,11 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>